<commit_message>
Changes in Create Call
</commit_message>
<xml_diff>
--- a/web-automation/src/test/java/com/fieldez/testdata/FieldezTestData.xlsx
+++ b/web-automation/src/test/java/com/fieldez/testdata/FieldezTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>test123</t>
   </si>
@@ -182,16 +182,106 @@
     <t>Tire4</t>
   </si>
   <si>
-    <t>Srinivas</t>
-  </si>
-  <si>
     <t>Remarks is there</t>
   </si>
   <si>
     <t>Amount For Line Item</t>
   </si>
   <si>
-    <t>Rs400</t>
+    <t>Rs600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City </t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Customer Last Name</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Ontoyo</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>Los Angeles Buckking Ham Street</t>
+  </si>
+  <si>
+    <t>New York USA</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Primary Number</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>stevel@jobs.co.in</t>
+  </si>
+  <si>
+    <t>Org Name</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Ottovia</t>
+  </si>
+  <si>
+    <t>Customer Type</t>
+  </si>
+  <si>
+    <t>Indiviual</t>
+  </si>
+  <si>
+    <t>WildCraft</t>
+  </si>
+  <si>
+    <t>Craft920393</t>
+  </si>
+  <si>
+    <t>ProductSerialNo</t>
+  </si>
+  <si>
+    <t>WarrantyType</t>
+  </si>
+  <si>
+    <t>SepcialInstructions</t>
+  </si>
+  <si>
+    <t>2  years</t>
+  </si>
+  <si>
+    <t>Warranty Type Bonues for  1 year</t>
+  </si>
+  <si>
+    <t>Do renewal after 3 years</t>
+  </si>
+  <si>
+    <t>ph-932883832</t>
+  </si>
+  <si>
+    <t>Customer Middle Name</t>
+  </si>
+  <si>
+    <t>Customer Id</t>
+  </si>
+  <si>
+    <t>cust883</t>
   </si>
 </sst>
 </file>
@@ -238,12 +328,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -634,36 +726,144 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="4" width="23" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="23" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="18.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="O1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
+      <c r="O2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -671,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -682,12 +882,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>